<commit_message>
SKlearn reSampling to balance the dataset, runs properly on Python version 3.12.3
</commit_message>
<xml_diff>
--- a/DatasetResults_MLP_SKLearn_reSample_14May24_2/Model_training_accuracy_and_evaluations_MLP with Attention layer_CardiacPrediction_(71142, 40)_Epoch_5.xlsx
+++ b/DatasetResults_MLP_SKLearn_reSample_14May24_2/Model_training_accuracy_and_evaluations_MLP with Attention layer_CardiacPrediction_(71142, 40)_Epoch_5.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,14 +434,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">           0       1.00      0.91      0.95      8889</t>
+          <t xml:space="preserve">           0       0.96      0.87      0.91      8889</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">           1       0.92      1.00      0.96      8897</t>
+          <t xml:space="preserve">           1       0.88      0.97      0.92      8897</t>
         </is>
       </c>
     </row>
@@ -451,21 +451,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    accuracy                           0.95     17786</t>
+          <t xml:space="preserve">    accuracy                           0.92     17786</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">   macro avg       0.96      0.95      0.95     17786</t>
+          <t xml:space="preserve">   macro avg       0.92      0.92      0.92     17786</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>weighted avg       0.96      0.95      0.95     17786</t>
+          <t>weighted avg       0.92      0.92      0.92     17786</t>
         </is>
       </c>
     </row>
@@ -488,27 +488,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[0.8411612510681152</t>
+          <t>[0.8054202198982239</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.917816162109375</t>
+          <t xml:space="preserve"> 0.864345133304596</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.9436989426612854</t>
+          <t xml:space="preserve"> 0.894369900226593</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.958355188369751</t>
+          <t xml:space="preserve"> 0.9108066558837891</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.9669203162193298]</t>
+          <t xml:space="preserve"> 0.9222955107688904]</t>
         </is>
       </c>
     </row>

</xml_diff>